<commit_message>
Add sample table (image)
</commit_message>
<xml_diff>
--- a/dns-monitor.xlsx
+++ b/dns-monitor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Development\PowerShell\DNSMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91F219F-FE1C-41E6-9700-CC46E3295166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8859960-342A-4112-9009-0EA8CA301CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -142,7 +142,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Gill Sans MT"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -150,13 +150,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Gill Sans MT"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Gill Sans MT"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -188,7 +188,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Gill Sans MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -201,10 +220,25 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C01362FB-BA52-4C2C-8B6B-15F050D1BA3D}" name="DNSChecks" displayName="DNSChecks" ref="A1:F14" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F14" xr:uid="{C01362FB-BA52-4C2C-8B6B-15F050D1BA3D}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{29B3BE3F-77F7-4ADF-849D-891081E67770}" name="DNS"/>
+    <tableColumn id="2" xr3:uid="{D92E8360-A896-40B5-9A85-C259749983DE}" name="Type"/>
+    <tableColumn id="3" xr3:uid="{A867871A-AAE9-4CFC-8211-A324FCB21178}" name="Find"/>
+    <tableColumn id="4" xr3:uid="{0C813479-0877-4D8D-AFFA-60408DB7C390}" name="Count"/>
+    <tableColumn id="5" xr3:uid="{167D57E6-4331-4F4E-A0F9-D5403D8A1928}" name="Match"/>
+    <tableColumn id="6" xr3:uid="{5E5F4D75-6F88-4EC5-818D-030F4648BE3F}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Dividend">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Dividend">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -212,83 +246,50 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="3D3D3D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EBEBEB"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4D1434"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="903163"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="B2324B"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="969FA7"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="66B1CE"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="40619D"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="828282"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Dividend">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Gill Sans MT" panose="020B0502020104020203"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Grek" typeface="Corbel"/>
+        <a:font script="Cyrl" typeface="Corbel"/>
+        <a:font script="Jpan" typeface="HGｺﾞｼｯｸE"/>
+        <a:font script="Hang" typeface="휴먼매직체"/>
+        <a:font script="Hans" typeface="华文中宋"/>
+        <a:font script="Hant" typeface="微軟正黑體"/>
+        <a:font script="Arab" typeface="Majalla UI"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Cordia New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -309,12 +310,49 @@
         <a:font script="Laoo" typeface="DokChampa"/>
         <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Viet" typeface="Tahoma"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Gill Sans MT" panose="020B0502020104020203"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Grek" typeface="Corbel"/>
+        <a:font script="Cyrl" typeface="Corbel"/>
+        <a:font script="Jpan" typeface="HGｺﾞｼｯｸE"/>
+        <a:font script="Hang" typeface="휴먼매직체"/>
+        <a:font script="Hans" typeface="华文中宋"/>
+        <a:font script="Hant" typeface="微軟正黑體"/>
+        <a:font script="Arab" typeface="Majalla UI"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Tahoma"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Dividend">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -323,23 +361,111 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="68000"/>
+                <a:alpha val="90000"/>
+                <a:lumMod val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="90000"/>
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:lumMod val="110000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="84000">
+              <a:schemeClr val="phClr">
+                <a:shade val="90000"/>
+                <a:lumMod val="88000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="rnd" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:lumMod val="90000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="rnd" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="55000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="88900" dist="38100" dir="5040000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="60000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="tl">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="38100" h="50800"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="90000"/>
+                <a:lumMod val="110000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="88000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="88000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -349,105 +475,21 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="90000"/>
+                <a:lumMod val="110000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="98000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="86000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="100000" b="100000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -456,7 +498,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Dividend" id="{9697A71B-4AB7-4A1A-BD5B-BB2D22835B57}" vid="{C21699FF-00E4-43C8-BBCC-D7E5536C3717}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -466,21 +508,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.625" customWidth="1"/>
+    <col min="4" max="5" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -500,7 +539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -517,7 +556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -531,7 +570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -551,7 +590,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -571,7 +610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -591,7 +630,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -611,7 +650,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -631,7 +670,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -648,7 +687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -665,7 +704,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -679,7 +718,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -696,7 +735,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -713,7 +752,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -730,6 +769,9 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>